<commit_message>
First Run with pycharm
Add pycharm datas
</commit_message>
<xml_diff>
--- a/Ontologie000.xlsx
+++ b/Ontologie000.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\RDFOWLTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\RDFOWLPY\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5196" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5196" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LisezMoi" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="DatatypeProperties" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -510,7 +509,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="78">
   <si>
     <t>URI</t>
   </si>
@@ -566,53 +565,21 @@
     <t>skos:preflabel  @en</t>
   </si>
   <si>
-    <t>skos:preflabel  %@fr</t>
-  </si>
-  <si>
-    <t>skos:preflabel  %@en</t>
-  </si>
-  <si>
     <t xml:space="preserve"> rdf:type  owl:Class</t>
   </si>
   <si>
-    <t xml:space="preserve"> rdfs:comment   % </t>
-  </si>
-  <si>
     <t>dc:contributor</t>
   </si>
   <si>
-    <t>% rdf:type owl:objectProperty</t>
-  </si>
-  <si>
-    <t>rdfs:domain  %</t>
-  </si>
-  <si>
-    <t>rdfs:range %</t>
-  </si>
-  <si>
-    <t>% rdf:type owl:DatatypePropery</t>
-  </si>
-  <si>
     <t>owl:minCardinality</t>
   </si>
   <si>
     <t>owl:maxCardinality</t>
   </si>
   <si>
-    <t xml:space="preserve">Ce tableur a pour but de renseigner les principaux éléments d'une modélisation métier afin de constituer rapidement une ontologie autorisant le raisonnement sur les données. 
-Des outils permettent de transformer ce tableau en une ontologie aux normes (en RDF/OWL  et en écriture texte de type Turtle pouvant être repris directement dans une  base de données RDF pour interrogation. 
-Un outil permet également de créer un tableau dérivé pouvant être repris directement dans un outillage de visualisation graphique pour observation et raisonnement. </t>
-  </si>
-  <si>
     <t>Conseil : commencer par les grandes entités métiers , poursuivre par les associations entre ces entités (ObjectProperties) et observer les résultats.</t>
   </si>
   <si>
-    <t>La majorité des champs sont optionnels. Par exemple, on peut très bien saisir les définitions des propriétés simples (DatatypeProperties) sans les associer forcément à une classe.</t>
-  </si>
-  <si>
-    <t>Les préfixes servent à simplifier l'écriture des identifiants uniques.</t>
-  </si>
-  <si>
     <t>ex:monOntologie</t>
   </si>
   <si>
@@ -670,9 +637,6 @@
     <t>drive</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>age</t>
   </si>
   <si>
@@ -716,6 +680,69 @@
   </si>
   <si>
     <t xml:space="preserve">  rdfs:subClassOf  </t>
+  </si>
+  <si>
+    <t>Les préfixes servent à simplifier l'écriture des identifiants uniques dans une représentation textuelle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prefix : onglet avec les préfixes standards. On y ajoute le préfixe des travaux courants. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ontology : simplement pour nommer le travail en cours. </t>
+  </si>
+  <si>
+    <t>Entities : description des objets métier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ObjectProperties : associations entre objets métier et cardinalités </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DatatypeProperties : attributs simple </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rdf:type owl:objectProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdfs:domain  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdfs:range </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rdfs:comment   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rdf:type owl:DatatypePropery</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rdfs:comment    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ce tableur a pour but de renseigner les principaux éléments d'une modélisation métier afin de constituer  une ontologie autorisant le raisonnement sur les données. </t>
+  </si>
+  <si>
+    <t>Onglets :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La majorité des champs sont optionnels : le monde descriptif est acceptable "ouvert" , cad que tout est autorisé tant qu'on n'a pas précisé les limites. </t>
+  </si>
+  <si>
+    <t>ex:Moto</t>
+  </si>
+  <si>
+    <t>Moto</t>
+  </si>
+  <si>
+    <t>ex:conduit</t>
+  </si>
+  <si>
+    <t>conduit</t>
+  </si>
+  <si>
+    <t>is driven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actuellement en train de conduire </t>
   </si>
 </sst>
 </file>
@@ -810,7 +837,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -852,9 +879,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -871,6 +895,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1188,7 +1218,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -1199,23 +1229,54 @@
     <col min="1" max="1" width="138.44140625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="16" customFormat="1" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" s="16" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>31</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1224,7 +1285,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1242,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1287,10 +1348,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>62</v>
+        <v>50</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1301,11 +1362,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+    <row r="10" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1330,9 +1391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1345,16 +1404,16 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
@@ -1362,24 +1421,24 @@
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="2" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
+    <row r="2" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
@@ -1401,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1418,7 +1477,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>16</v>
@@ -1427,72 +1486,85 @@
         <v>17</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="B4" s="21" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="C4" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="D5" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>54</v>
+      <c r="E5" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="21" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1504,19 +1576,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="23" style="12" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="12" customWidth="1"/>
-    <col min="5" max="5" width="18" style="12" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="59.5546875" customWidth="1"/>
     <col min="7" max="7" width="16.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.21875" style="5" bestFit="1" customWidth="1"/>
@@ -1524,54 +1596,76 @@
   <sheetData>
     <row r="1" spans="1:8" s="13" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="F1" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+    </row>
+    <row r="2" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="22">
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+    </row>
+    <row r="3" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="21">
         <v>0</v>
       </c>
-      <c r="H2" s="22" t="s">
-        <v>52</v>
+      <c r="H3" s="21">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1585,12 +1679,12 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.77734375" customWidth="1"/>
@@ -1602,53 +1696,53 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="22">
+    </row>
+    <row r="2" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="21">
         <v>1</v>
       </c>
-      <c r="H2" s="22">
+      <c r="H2" s="21">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajout type de lien
avec  mise à jour du ppt
</commit_message>
<xml_diff>
--- a/Ontologie000.xlsx
+++ b/Ontologie000.xlsx
@@ -1579,7 +1579,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1661,9 +1661,7 @@
       <c r="F3" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="21">
-        <v>0</v>
-      </c>
+      <c r="G3" s="21"/>
       <c r="H3" s="21">
         <v>1</v>
       </c>

</xml_diff>